<commit_message>
#add save note field to stock_goods
</commit_message>
<xml_diff>
--- a/Document/5.Reference/191003_ThanhThuy_DanhSachSuaDoi_NoiBo.xlsx
+++ b/Document/5.Reference/191003_ThanhThuy_DanhSachSuaDoi_NoiBo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FED8C4-4BF9-44E8-87F3-1B0DE02BE0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40DE219-FCC0-42B2-B07C-4B3A11FA0DFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,22 +662,22 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="48.08984375" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -713,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -733,7 +733,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -755,7 +755,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -779,7 +779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="159" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -823,7 +823,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>

</xml_diff>